<commit_message>
Continued Task A: Meta Info
</commit_message>
<xml_diff>
--- a/_Assets/Meta Info.xlsx
+++ b/_Assets/Meta Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WhaleplaneStudios\FinanceRun\_Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9F9F49-074F-4167-96AF-41DBD04250AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367736D0-CF33-4AA1-A854-47BBD265AD81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="5640" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
@@ -29,15 +29,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Player</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+  <si>
+    <t>Enemy Name</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Home Repairs</t>
+  </si>
+  <si>
+    <t>Groceries</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>Car Insurance</t>
+  </si>
+  <si>
+    <t>Water Bill</t>
+  </si>
+  <si>
+    <t>Heating Bill</t>
+  </si>
+  <si>
+    <t>Electricity Bill</t>
+  </si>
+  <si>
+    <t>Roof Damage</t>
+  </si>
+  <si>
+    <t>Flood Damage</t>
+  </si>
+  <si>
+    <t>Renovations</t>
+  </si>
+  <si>
+    <t>Player Defense</t>
+  </si>
+  <si>
+    <t>Defense Stat</t>
+  </si>
+  <si>
+    <t>Hobbies</t>
+  </si>
+  <si>
+    <t>Holiday Shopping</t>
+  </si>
+  <si>
+    <t>Full Tank</t>
+  </si>
+  <si>
+    <t>Vehicle Costs</t>
+  </si>
+  <si>
+    <t>New Tires</t>
+  </si>
+  <si>
+    <t>Car Repairs</t>
+  </si>
+  <si>
+    <t>Appliance Replacement</t>
+  </si>
+  <si>
+    <t>Occurrence</t>
+  </si>
+  <si>
+    <t>Last Room</t>
+  </si>
+  <si>
+    <t>First 2 and last 2 Rooms</t>
+  </si>
+  <si>
+    <t>Every Room</t>
+  </si>
+  <si>
+    <t>Only one Room</t>
+  </si>
+  <si>
+    <t>Twice per Room</t>
+  </si>
+  <si>
+    <t>Two Rooms</t>
+  </si>
+  <si>
+    <t>Once per room</t>
+  </si>
+  <si>
+    <t>Stat Average $</t>
+  </si>
+  <si>
+    <t>Three Rooms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,9 +168,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,22 +452,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -383,13 +498,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED84013-CBCA-42C9-BE32-D2CFD301BAC5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>900</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2500</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>1600</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>1350</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>250</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2">
+        <v>700</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2">
+        <v>800</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1500</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -399,7 +705,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -411,7 +717,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -423,7 +729,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished Task A: Meta Info
Filled out all meta info in .xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/_Assets/Meta Info.xlsx
+++ b/_Assets/Meta Info.xlsx
@@ -1,35 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WhaleplaneStudios\FinanceRun\_Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367736D0-CF33-4AA1-A854-47BBD265AD81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D1899F-EF62-4AA8-BB5B-DD72BCEC0CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
     <sheet name="Enemies" sheetId="2" r:id="rId2"/>
     <sheet name="Items" sheetId="3" r:id="rId3"/>
     <sheet name="Vehicles" sheetId="4" r:id="rId4"/>
-    <sheet name="Education" sheetId="5" r:id="rId5"/>
+    <sheet name="Jobs" sheetId="6" r:id="rId5"/>
+    <sheet name="Education" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="97">
   <si>
     <t>Enemy Name</t>
   </si>
@@ -122,6 +132,204 @@
   </si>
   <si>
     <t>Three Rooms</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Stat</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Salary Increase</t>
+  </si>
+  <si>
+    <t>Utility Waiver</t>
+  </si>
+  <si>
+    <t>Remove total utility cost</t>
+  </si>
+  <si>
+    <t>Efficiency Boost</t>
+  </si>
+  <si>
+    <t>Remove one hit</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Uncommon</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>Enemy Type</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Adds $500 to player money</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Lucky Day</t>
+  </si>
+  <si>
+    <t>Remove total cost</t>
+  </si>
+  <si>
+    <t>Remove total repair cost</t>
+  </si>
+  <si>
+    <t>Total Repair Kit</t>
+  </si>
+  <si>
+    <t>Toolbox</t>
+  </si>
+  <si>
+    <t>Gift Card</t>
+  </si>
+  <si>
+    <t>Generous Gift</t>
+  </si>
+  <si>
+    <t>Remove total shopping cost</t>
+  </si>
+  <si>
+    <t>Remove one shopping cost</t>
+  </si>
+  <si>
+    <t>Incredible Gift</t>
+  </si>
+  <si>
+    <t>Adds $1000 to player money</t>
+  </si>
+  <si>
+    <t>Universal Coupon</t>
+  </si>
+  <si>
+    <t>Remove total vehicle cost</t>
+  </si>
+  <si>
+    <t>Remove one vehicle cost</t>
+  </si>
+  <si>
+    <t>Store Coupon</t>
+  </si>
+  <si>
+    <t>Mechanical Waiver</t>
+  </si>
+  <si>
+    <t>Rusty Coupon</t>
+  </si>
+  <si>
+    <t>15 Vexus Vortex</t>
+  </si>
+  <si>
+    <t>98 Tord Rustang</t>
+  </si>
+  <si>
+    <t>08 Coyota Roccola</t>
+  </si>
+  <si>
+    <t>20 Berrari "The Berrari"</t>
+  </si>
+  <si>
+    <t>Accountant</t>
+  </si>
+  <si>
+    <t>Increased Stat</t>
+  </si>
+  <si>
+    <t>Secretary</t>
+  </si>
+  <si>
+    <t>Farmer</t>
+  </si>
+  <si>
+    <t>Mechanical Engineer</t>
+  </si>
+  <si>
+    <t>Graphic Design</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Electrician</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Lawyer</t>
+  </si>
+  <si>
+    <t>Dentist</t>
+  </si>
+  <si>
+    <t>4-Year College</t>
+  </si>
+  <si>
+    <t>2-Year College</t>
+  </si>
+  <si>
+    <t>Trade School</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Culinary School</t>
+  </si>
+  <si>
+    <t>4y + Medical School</t>
+  </si>
+  <si>
+    <t>4y + Law School</t>
+  </si>
+  <si>
+    <t>4y + Dental School</t>
   </si>
 </sst>
 </file>
@@ -168,10 +376,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,38 +663,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -500,19 +709,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED84013-CBCA-42C9-BE32-D2CFD301BAC5}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -527,7 +736,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -541,7 +750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -552,7 +761,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -563,7 +772,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -577,7 +786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -588,7 +797,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -599,7 +808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -610,7 +819,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -624,7 +833,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -635,7 +844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -646,7 +855,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -660,7 +869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -671,7 +880,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -682,7 +891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -701,36 +910,710 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FAD134C-3A3F-459E-A49F-A1CC3869EBB6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED09784-53D8-4051-A905-93C8A6EE9495}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C2">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="2">
+        <v>25000</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="2">
+        <v>56000</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C5">
+        <v>-20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B04006D-9884-4910-9EA7-340C38FBA833}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2">
+        <v>51000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="2">
+        <v>26000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="2">
+        <v>71000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="2">
+        <v>74000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="2">
+        <v>46000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="2">
+        <v>24000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="2">
+        <v>294000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="2">
+        <v>86000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="2">
+        <v>85000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="2">
+        <v>166000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78896DF-ED2C-4894-995F-B0ECFBFB0D19}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="2">
+        <v>34000</v>
+      </c>
+      <c r="D2" s="2">
+        <v>70000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="2">
+        <v>14000</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="2">
+        <v>34000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="2">
+        <v>34000</v>
+      </c>
+      <c r="D6" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="2">
+        <v>34000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="2">
+        <v>34000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="2">
+        <v>30000</v>
+      </c>
+      <c r="D10" s="2">
+        <v>25000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="2">
+        <v>90000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="2">
+        <v>34000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="2">
+        <v>80000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="2">
+        <v>80000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Task H: Vehicle Menu
Confirming vehicle saves both player stat and payment, payment is taken after each room is loaded. Game also pauses at a different camera angle while the intro menu for each room is open.
</commit_message>
<xml_diff>
--- a/_Assets/Meta Info.xlsx
+++ b/_Assets/Meta Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WhaleplaneStudios\FinanceRun\_Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D1899F-EF62-4AA8-BB5B-DD72BCEC0CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA1BD47-5C0B-4AA3-9E3F-A7961C952019}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="96">
   <si>
     <t>Enemy Name</t>
   </si>
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t>08 Coyota Roccola</t>
-  </si>
-  <si>
-    <t>20 Berrari "The Berrari"</t>
   </si>
   <si>
     <t>Accountant</t>
@@ -663,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1116,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED09784-53D8-4051-A905-93C8A6EE9495}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1171,15 +1168,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="2">
-        <v>300000</v>
-      </c>
-      <c r="C5">
-        <v>-20</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1209,12 +1198,12 @@
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2">
         <v>51000</v>
@@ -1225,7 +1214,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2">
         <v>26000</v>
@@ -1236,7 +1225,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <v>43000</v>
@@ -1247,7 +1236,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2">
         <v>71000</v>
@@ -1258,7 +1247,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="2">
         <v>45000</v>
@@ -1269,7 +1258,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="2">
         <v>74000</v>
@@ -1280,7 +1269,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2">
         <v>46000</v>
@@ -1291,7 +1280,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="2">
         <v>45000</v>
@@ -1302,7 +1291,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="2">
         <v>24000</v>
@@ -1313,7 +1302,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="2">
         <v>294000</v>
@@ -1324,7 +1313,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="2">
         <v>86000</v>
@@ -1335,7 +1324,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="2">
         <v>85000</v>
@@ -1346,7 +1335,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="2">
         <v>166000</v>
@@ -1389,15 +1378,15 @@
         <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2">
         <v>34000</v>
@@ -1406,15 +1395,15 @@
         <v>70000</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="2">
         <v>14000</v>
@@ -1423,7 +1412,7 @@
         <v>10000</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1431,7 +1420,7 @@
         <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
         <v>49</v>
@@ -1445,10 +1434,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2">
         <v>34000</v>
@@ -1457,15 +1446,15 @@
         <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2">
         <v>34000</v>
@@ -1474,15 +1463,15 @@
         <v>15000</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="2">
         <v>34000</v>
@@ -1491,15 +1480,15 @@
         <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2">
         <v>7000</v>
@@ -1508,15 +1497,15 @@
         <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2">
         <v>34000</v>
@@ -1525,15 +1514,15 @@
         <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="2">
         <v>30000</v>
@@ -1542,15 +1531,15 @@
         <v>25000</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="2">
         <v>90000</v>
@@ -1559,15 +1548,15 @@
         <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="2">
         <v>34000</v>
@@ -1576,15 +1565,15 @@
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="2">
         <v>80000</v>
@@ -1593,15 +1582,15 @@
         <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="2">
         <v>80000</v>
@@ -1610,7 +1599,7 @@
         <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Task I: Education Menu
Most functionality borrowed from vehicle menu, can refuse higher education, has static interest rate
</commit_message>
<xml_diff>
--- a/_Assets/Meta Info.xlsx
+++ b/_Assets/Meta Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WhaleplaneStudios\FinanceRun\_Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA1BD47-5C0B-4AA3-9E3F-A7961C952019}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C596EF-9B8E-4D49-A9C3-91FB87E5870C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1114,7 +1114,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1142,7 +1142,7 @@
         <v>10000</v>
       </c>
       <c r="C2">
-        <v>-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Finished Task L: Enemy Combat
Renamed variables and messages for actual R/P/S finance names (knowledge, preparation and skill instead of rock, paper, and scissors). Weighted damage taken by player based on comparing stat to enemy stat. Created subclasses for each specific enemy type and put them into the rooms specified by meta info.xlsx
</commit_message>
<xml_diff>
--- a/_Assets/Meta Info.xlsx
+++ b/_Assets/Meta Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WhaleplaneStudios\FinanceRun\_Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C596EF-9B8E-4D49-A9C3-91FB87E5870C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D31EE9-674A-4FB2-BC27-1DDCC5969B0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="119">
   <si>
     <t>Enemy Name</t>
   </si>
@@ -77,21 +77,12 @@
     <t>Renovations</t>
   </si>
   <si>
-    <t>Player Defense</t>
-  </si>
-  <si>
-    <t>Defense Stat</t>
-  </si>
-  <si>
     <t>Hobbies</t>
   </si>
   <si>
     <t>Holiday Shopping</t>
   </si>
   <si>
-    <t>Full Tank</t>
-  </si>
-  <si>
     <t>Vehicle Costs</t>
   </si>
   <si>
@@ -107,33 +98,6 @@
     <t>Occurrence</t>
   </si>
   <si>
-    <t>Last Room</t>
-  </si>
-  <si>
-    <t>First 2 and last 2 Rooms</t>
-  </si>
-  <si>
-    <t>Every Room</t>
-  </si>
-  <si>
-    <t>Only one Room</t>
-  </si>
-  <si>
-    <t>Twice per Room</t>
-  </si>
-  <si>
-    <t>Two Rooms</t>
-  </si>
-  <si>
-    <t>Once per room</t>
-  </si>
-  <si>
-    <t>Stat Average $</t>
-  </si>
-  <si>
-    <t>Three Rooms</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -327,6 +291,111 @@
   </si>
   <si>
     <t>4y + Dental School</t>
+  </si>
+  <si>
+    <t>Knowledge</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Preparation</t>
+  </si>
+  <si>
+    <t>Initial $</t>
+  </si>
+  <si>
+    <t>Tank of Gas</t>
+  </si>
+  <si>
+    <t>Player stats in increments of 5 from 0 to 20</t>
+  </si>
+  <si>
+    <t>Vehicle adds to preparation stat</t>
+  </si>
+  <si>
+    <t>Enemy stats in increments of 5 from 0 to 15</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>Scissors</t>
+  </si>
+  <si>
+    <t>Win Message</t>
+  </si>
+  <si>
+    <t>Loss Message</t>
+  </si>
+  <si>
+    <t>Player Attacks</t>
+  </si>
+  <si>
+    <t>R/P/S Equivalent</t>
+  </si>
+  <si>
+    <t>You attacked with KNOWLEDGE, which overcame the enemy's SKILL</t>
+  </si>
+  <si>
+    <t>You attacked with PREPARATION, which overcame the enemy's KNOWLEDGE</t>
+  </si>
+  <si>
+    <t>You attacked with SKILL, which overcame the enemy's PREPARATION</t>
+  </si>
+  <si>
+    <t>The enemy defended with PREPARATION, which overcame your KNOWLEDGE</t>
+  </si>
+  <si>
+    <t>The enemy defended with SKILL, which overcame your PREPARATION</t>
+  </si>
+  <si>
+    <t>The enemy defended with KNOWLEDGE, which overcame your SKILL</t>
+  </si>
+  <si>
+    <t>Formula (initial is actually initial/3):</t>
+  </si>
+  <si>
+    <t>if enemy stat &gt;= player stat</t>
+  </si>
+  <si>
+    <t>Damage to player = Initial $ - (player stat% - enemy stat%)</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>Damage = 1000 + (10 - 5)% = 1200</t>
+  </si>
+  <si>
+    <t>Damage = 1000 - (15 - 10)% =  800</t>
+  </si>
+  <si>
+    <t>Damage to player = Initial $ + (enemy stat% - player stat%)</t>
+  </si>
+  <si>
+    <t>1 2 3 4 5 6 7 8 9 10</t>
+  </si>
+  <si>
+    <t>1 2 9 10</t>
+  </si>
+  <si>
+    <t>(x2) 2 3 4 5 6 7 8 9 10</t>
+  </si>
+  <si>
+    <t>6 8</t>
+  </si>
+  <si>
+    <t>4 8</t>
+  </si>
+  <si>
+    <t>5 7 10</t>
+  </si>
+  <si>
+    <t>2 4 6 8 10</t>
   </si>
 </sst>
 </file>
@@ -373,11 +442,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,42 +733,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.08984375" customWidth="1"/>
     <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="3" width="67.6328125" customWidth="1"/>
+    <col min="4" max="4" width="73.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -704,202 +826,373 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED84013-CBCA-42C9-BE32-D2CFD301BAC5}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="21.6328125" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="C2">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C3">
         <v>70</v>
       </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="C4">
         <v>110</v>
       </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
         <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>7</v>
       </c>
       <c r="C5">
         <v>900</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>10</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5">
+        <v>9</v>
       </c>
       <c r="C6">
         <v>2500</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>11</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10</v>
       </c>
       <c r="C7">
         <v>1600</v>
       </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="C8">
         <v>1350</v>
       </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>112</v>
       </c>
       <c r="C9" s="2">
         <v>250</v>
       </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="C10" s="2">
         <v>100</v>
       </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>15</v>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10</v>
       </c>
       <c r="C11" s="2">
         <v>1000</v>
       </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="C12" s="2">
         <v>50</v>
       </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="C13" s="2">
         <v>700</v>
       </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>18</v>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5">
+        <v>9</v>
       </c>
       <c r="C14" s="2">
         <v>800</v>
       </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="C15" s="2">
         <v>1500</v>
       </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="F19:J19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -923,184 +1216,184 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1113,7 +1406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED09784-53D8-4051-A905-93C8A6EE9495}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1125,18 +1418,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2">
         <v>10000</v>
@@ -1147,7 +1440,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2">
         <v>25000</v>
@@ -1158,7 +1451,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2">
         <v>56000</v>
@@ -1192,18 +1485,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2">
         <v>51000</v>
@@ -1214,29 +1507,29 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2">
         <v>26000</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2">
         <v>43000</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2">
         <v>71000</v>
@@ -1247,29 +1540,29 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2">
         <v>45000</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2">
         <v>74000</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2">
         <v>46000</v>
@@ -1280,68 +1573,68 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2">
         <v>45000</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B10" s="2">
         <v>24000</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B11" s="2">
         <v>294000</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2">
         <v>86000</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B13" s="2">
         <v>85000</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B14" s="2">
         <v>166000</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1366,27 +1659,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2">
         <v>34000</v>
@@ -1395,15 +1688,15 @@
         <v>70000</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2">
         <v>14000</v>
@@ -1412,49 +1705,49 @@
         <v>10000</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2">
         <v>34000</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2">
         <v>34000</v>
@@ -1463,66 +1756,66 @@
         <v>15000</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2">
         <v>34000</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C8" s="2">
         <v>7000</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2">
         <v>34000</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2">
         <v>30000</v>
@@ -1531,75 +1824,75 @@
         <v>25000</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C11" s="2">
         <v>90000</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C12" s="2">
         <v>34000</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2">
         <v>80000</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C14" s="2">
         <v>80000</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started 2O: Random Job Selection
Updated meta info spreadsheet, created struct and data table for access to all info in-engine
</commit_message>
<xml_diff>
--- a/_Assets/Meta Info.xlsx
+++ b/_Assets/Meta Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WhaleplaneStudios\FinanceRun\_Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D31EE9-674A-4FB2-BC27-1DDCC5969B0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE365FE-140A-4D6A-AC7D-6B5A263BC7B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="1260" windowWidth="17280" windowHeight="10392" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="119">
   <si>
     <t>Enemy Name</t>
   </si>
@@ -442,16 +442,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,15 +749,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
-    <col min="3" max="3" width="67.6328125" customWidth="1"/>
-    <col min="4" max="4" width="73.6328125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
+    <col min="4" max="4" width="73.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -761,7 +771,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -775,7 +785,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -789,7 +799,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -803,17 +813,17 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -828,21 +838,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED84013-CBCA-42C9-BE32-D2CFD301BAC5}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.81640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +872,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -882,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -902,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -922,11 +932,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>7</v>
       </c>
       <c r="C5">
@@ -942,11 +952,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>9</v>
       </c>
       <c r="C6">
@@ -962,11 +972,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>10</v>
       </c>
       <c r="C7">
@@ -982,7 +992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1002,7 +1012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1022,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1042,11 +1052,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>10</v>
       </c>
       <c r="C11" s="2">
@@ -1062,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -1082,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1102,11 +1112,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>9</v>
       </c>
       <c r="C14" s="2">
@@ -1122,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1142,48 +1152,48 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
   </sheetData>
@@ -1206,15 +1216,15 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1228,7 +1238,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1242,7 +1252,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1256,7 +1266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1270,7 +1280,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1284,7 +1294,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1298,7 +1308,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1312,7 +1322,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1326,7 +1336,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1340,7 +1350,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1368,7 +1378,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1382,7 +1392,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1410,13 +1420,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1427,7 +1437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
@@ -1438,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1449,7 +1459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1460,7 +1470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
     </row>
   </sheetData>
@@ -1470,20 +1480,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B04006D-9884-4910-9EA7-340C38FBA833}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1491,10 +1504,22 @@
         <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1502,10 +1527,22 @@
         <v>51000</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="2">
+        <v>34000</v>
+      </c>
+      <c r="F2" s="7">
+        <v>70000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1513,10 +1550,22 @@
         <v>26000</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="2">
+        <v>14000</v>
+      </c>
+      <c r="F3" s="7">
+        <v>10000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1524,10 +1573,22 @@
         <v>43000</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7000</v>
+      </c>
+      <c r="F4" s="8">
+        <v>15000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1535,10 +1596,22 @@
         <v>71000</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="2">
+        <v>34000</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1546,10 +1619,22 @@
         <v>45000</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="2">
+        <v>34000</v>
+      </c>
+      <c r="F6" s="7">
+        <v>15000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -1557,10 +1642,22 @@
         <v>74000</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="2">
+        <v>34000</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1568,10 +1665,22 @@
         <v>46000</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7000</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -1579,10 +1688,22 @@
         <v>45000</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="2">
+        <v>34000</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1590,10 +1711,22 @@
         <v>24000</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="2">
+        <v>30000</v>
+      </c>
+      <c r="F10" s="7">
+        <v>25000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -1601,10 +1734,22 @@
         <v>294000</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="2">
+        <v>90000</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -1612,10 +1757,22 @@
         <v>86000</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="2">
+        <v>34000</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1623,10 +1780,22 @@
         <v>85000</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="2">
+        <v>80000</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -1634,6 +1803,18 @@
         <v>166000</v>
       </c>
       <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="2">
+        <v>80000</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1646,18 +1827,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78896DF-ED2C-4894-995F-B0ECFBFB0D19}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.36328125" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -1674,7 +1855,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1691,7 +1872,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1708,24 +1889,24 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
+      <c r="C4" s="2">
+        <v>7000</v>
+      </c>
+      <c r="D4" s="5">
+        <v>15000</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1742,7 +1923,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1759,7 +1940,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -1776,7 +1957,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -1793,7 +1974,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -1810,7 +1991,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -1827,7 +2008,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -1844,7 +2025,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -1861,7 +2042,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -1878,7 +2059,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>

</xml_diff>